<commit_message>
added new data cleaning version
</commit_message>
<xml_diff>
--- a/Kevin/Data_Cleaning.xlsx
+++ b/Kevin/Data_Cleaning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuhai\Desktop\NYCDSA_Boot_Camp\Projects\Housing_ML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuhai\Desktop\NYCDSA_Boot_Camp\Projects\Kaggle-House-Prices\Kevin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3D2058-E8DB-4035-9623-2C6CD9E30555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8DC0784-0977-4536-8C49-D08956CCBE83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{81F687DA-82C1-49D9-A9E6-94A695FADD8F}"/>
+    <workbookView xWindow="83" yWindow="0" windowWidth="13680" windowHeight="9532" xr2:uid="{81F687DA-82C1-49D9-A9E6-94A695FADD8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Missing_Value" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Improve_of_existing_feature" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -914,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C041F5E-5072-4E39-BCA5-BFBC02CD58A7}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1444,7 +1445,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1825,14 +1826,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F2AC05-2915-42F8-8F8A-4764922CFF0F}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.3984375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>